<commit_message>
check bao cao và CTKM
</commit_message>
<xml_diff>
--- a/Api.ManagerGift/DownloadWordExcel/Báo cáo nhập kho 2020.xlsx
+++ b/Api.ManagerGift/DownloadWordExcel/Báo cáo nhập kho 2020.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
@@ -16,12 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>BÁO CÁO QUÀ TẶNG NHẬP KHO</t>
   </si>
   <si>
-    <t>Từ ngày 2018-04-06, Đến ngày 2020-04-06</t>
+    <t>Từ ngày 2020-03-29, Đến ngày 2020-04-08</t>
   </si>
   <si>
     <t>STT</t>
@@ -60,25 +60,19 @@
     <t>1</t>
   </si>
   <si>
-    <t>QT Hộ kinh doanh</t>
-  </si>
-  <si>
-    <t>KH-kinhdoanh</t>
-  </si>
-  <si>
-    <t>14</t>
+    <t>Detox</t>
+  </si>
+  <si>
+    <t>DT</t>
   </si>
   <si>
     <t>bo</t>
   </si>
   <si>
-    <t>50000.0000</t>
-  </si>
-  <si>
-    <t>700000.0000</t>
-  </si>
-  <si>
-    <t>04-02-2020</t>
+    <t>4500000.0000</t>
+  </si>
+  <si>
+    <t>01-04-2020</t>
   </si>
   <si>
     <t>P. Quản lý bán hàng</t>
@@ -90,124 +84,13 @@
     <t>2</t>
   </si>
   <si>
-    <t>Detox</t>
-  </si>
-  <si>
-    <t>DT</t>
-  </si>
-  <si>
-    <t>4500000.0000</t>
-  </si>
-  <si>
-    <t>01-04-2020</t>
+    <t>Quyen</t>
+  </si>
+  <si>
+    <t>QQ</t>
   </si>
   <si>
     <t>3</t>
-  </si>
-  <si>
-    <t>Ngọc Trinh</t>
-  </si>
-  <si>
-    <t>NTXD</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>lô</t>
-  </si>
-  <si>
-    <t>500000.0000</t>
-  </si>
-  <si>
-    <t>50500000.0000</t>
-  </si>
-  <si>
-    <t>23-03-2020</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Móc chìa khóa samsung</t>
-  </si>
-  <si>
-    <t>MK_SS</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>Cái</t>
-  </si>
-  <si>
-    <t>35000.0000</t>
-  </si>
-  <si>
-    <t>70000000.0000</t>
-  </si>
-  <si>
-    <t>22-11-2019</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Móc chìa khóa iphone</t>
-  </si>
-  <si>
-    <t>MK_IP</t>
-  </si>
-  <si>
-    <t>1500</t>
-  </si>
-  <si>
-    <t>75000000.0000</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Mũ bảo hiểm iphone</t>
-  </si>
-  <si>
-    <t>MBH_IP</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>180000.0000</t>
-  </si>
-  <si>
-    <t>27000000.0000</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Mũ bảo hiểm samsung</t>
-  </si>
-  <si>
-    <t>MBH_SS</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>150000.0000</t>
-  </si>
-  <si>
-    <t>45000000.0000</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Quyen</t>
-  </si>
-  <si>
-    <t>QQ</t>
   </si>
   <si>
     <t>200000.0000</t>
@@ -792,7 +675,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AF528D-71AB-4BC7-9A2D-A451951AFBDC}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="E16" sqref="E16"/>
@@ -900,292 +783,82 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="15.75">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="15.75">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>22</v>
-      </c>
+    <row r="7" s="2" customFormat="1" ht="15.75"/>
+    <row r="8" spans="1:2" s="2" customFormat="1" ht="15.75">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="15.75">
-      <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>22</v>
-      </c>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="15.75">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" ht="15.75">
-      <c r="A9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="15.75">
-      <c r="A10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" ht="15.75">
-      <c r="A11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" ht="15.75">
-      <c r="A12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" s="2" customFormat="1" ht="15.75"/>
-    <row r="14" spans="1:2" s="2" customFormat="1" ht="15.75">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="15.75">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" s="2" customFormat="1" ht="15.75"/>
+    <row r="10" s="2" customFormat="1" ht="15.75"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:K1"/>
@@ -1206,7 +879,7 @@
   <sheetData>
     <row r="5" spans="1:1" ht="23.25" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>